<commit_message>
Update DR# 722 AllHome (Cleaning Cards and Ribbons)_02_16_2022.xlsx
</commit_message>
<xml_diff>
--- a/DR# 722 AllHome (Cleaning Cards and Ribbons)_02_16_2022.xlsx
+++ b/DR# 722 AllHome (Cleaning Cards and Ribbons)_02_16_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaime Ponio IV\Documents\GitHub\Delivery-Receipt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C415287-DD05-4D36-8DFA-2E8572C20895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0F1734-6463-463F-9DF0-733AF330E236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -138,9 +138,6 @@
     <t>Address: South Super Highway, Alabang, Muntinlupa, Metro Manila</t>
   </si>
   <si>
-    <t>TO:  AllHome</t>
-  </si>
-  <si>
     <t>Cleaning Cards</t>
   </si>
   <si>
@@ -174,6 +171,9 @@
       </rPr>
       <t xml:space="preserve"> 000722</t>
     </r>
+  </si>
+  <si>
+    <t>TO:  AllDay</t>
   </si>
 </sst>
 </file>
@@ -1373,7 +1373,7 @@
   <dimension ref="A2:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1428,12 +1428,12 @@
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
       <c r="E9" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="21" customHeight="1">
       <c r="A10" s="26" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -1494,10 +1494,10 @@
     </row>
     <row r="15" spans="1:13" ht="18.75">
       <c r="A15" s="43" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="37">
         <v>20</v>
@@ -1511,10 +1511,10 @@
     </row>
     <row r="16" spans="1:13" ht="18.75">
       <c r="A16" s="43" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="29">
         <v>20</v>

</xml_diff>